<commit_message>
Move from tab delimited .csvs to .xlsx for easy reading of data. Couple of options for more flexibility with F0AM added.
</commit_message>
<xml_diff>
--- a/Data/Functional_Group_SMARTs.xlsx
+++ b/Data/Functional_Group_SMARTs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3be239a439bc7664/Documents/Research/Projects/MIT/pOrgNO3/code/MCM_RCIM_SMILES/python/MCM_web_scraper/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3be239a439bc7664/Documents/Research/Projects/MIT/pOrgNO3/code/MCM_RCIM_SMILES/python/pyMCM/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C4F3C4E-712A-4552-94B7-A2C1FF83A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{8C4F3C4E-712A-4552-94B7-A2C1FF83A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B33E8E32-FC42-48E8-8E52-69E3A013834D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{D7025BAE-6866-4008-AAF2-D095803B35C8}"/>
+    <workbookView xWindow="35565" yWindow="930" windowWidth="19125" windowHeight="11835" xr2:uid="{D7025BAE-6866-4008-AAF2-D095803B35C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -509,7 +509,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -517,13 +517,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,542 +854,653 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D5DD2E-B490-4337-94AA-58F9A68F8510}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="55.140625" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" customWidth="1"/>
+    <col min="4" max="4" width="51.140625" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>41</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>42</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>46</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>48</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>50</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>52</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>53</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>54</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>56</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>57</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>58</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>60</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>61</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>62</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>63</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>65</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>66</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>67</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>68</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
         <v>70</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>71</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>72</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>73</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
         <v>75</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>76</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>77</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>78</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
         <v>80</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>81</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>82</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>83</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
         <v>85</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>86</v>
-      </c>
-      <c r="C22" t="s">
-        <v>87</v>
       </c>
       <c r="D22" t="s">
         <v>87</v>
       </c>
       <c r="E22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
         <v>89</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>90</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
         <v>92</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>93</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>146</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>95</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>96</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>97</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>98</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>100</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>101</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>102</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
         <v>104</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>105</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>106</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>107</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
         <v>109</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>110</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>111</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>112</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
         <v>114</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>115</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>116</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
         <v>118</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>119</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>120</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
         <v>122</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>123</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>124</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
         <v>125</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>126</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
         <v>128</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>129</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
         <v>131</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>132</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
         <v>134</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>135</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
         <v>137</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>138</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
         <v>140</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>141</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
         <v>143</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>144</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to F0AM tools
</commit_message>
<xml_diff>
--- a/Data/Functional_Group_SMARTs.xlsx
+++ b/Data/Functional_Group_SMARTs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3be239a439bc7664/Documents/Research/Projects/MIT/pOrgNO3/code/MCM_RCIM_SMILES/python/pyMCM/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{8C4F3C4E-712A-4552-94B7-A2C1FF83A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B33E8E32-FC42-48E8-8E52-69E3A013834D}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{8C4F3C4E-712A-4552-94B7-A2C1FF83A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF2DC0EE-FA1E-4674-8A2A-3EC33138F8E7}"/>
   <bookViews>
-    <workbookView xWindow="35565" yWindow="930" windowWidth="19125" windowHeight="11835" xr2:uid="{D7025BAE-6866-4008-AAF2-D095803B35C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{D7025BAE-6866-4008-AAF2-D095803B35C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="154">
   <si>
     <t>Name</t>
   </si>
@@ -478,6 +478,24 @@
   </si>
   <si>
     <t xml:space="preserve">Its a "find all the rest" string. Tends to be mostly aromatic alchols that aren't phenols in the MCM. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Tertiary_NO3s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catches a NO3 attached to a C that is ONLY attached to other Cs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For ppl who care about hydrolysis… </t>
+  </si>
+  <si>
+    <t>[$([#7X3](=[#8X1])(=[#8X1])([#8]-[#6X4H0])),$([#7X3+]([#8X1-])(=[#8X1])([#8]-[#6X4H0]))]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does NOT catch acyl RO2s… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does NOT catch acyl ROs… </t>
   </si>
 </sst>
 </file>
@@ -854,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D5DD2E-B490-4337-94AA-58F9A68F8510}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,6 +935,9 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
+      <c r="E3" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -931,6 +952,9 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
+      <c r="E4" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -996,16 +1020,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>151</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>149</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1013,16 +1037,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1030,13 +1054,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1044,19 +1071,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1064,16 +1085,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1081,16 +1105,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1098,16 +1122,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1115,16 +1139,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1132,19 +1156,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1152,19 +1173,19 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1172,19 +1193,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1192,19 +1213,19 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1212,19 +1233,19 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F21" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1232,19 +1253,19 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E22" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1252,13 +1273,19 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="E23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1266,16 +1293,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
-      </c>
-      <c r="E24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1283,19 +1307,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1303,16 +1324,19 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="F26" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1320,19 +1344,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
-      </c>
-      <c r="F27" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1340,19 +1361,19 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D28" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E28" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F28" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1360,16 +1381,19 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D29" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E29" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="F29" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1377,16 +1401,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E30" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1394,16 +1418,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C31" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E31" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1411,13 +1435,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D32" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="E32" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1425,13 +1452,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D33" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1439,13 +1466,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C34" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1453,13 +1480,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1467,13 +1494,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D36" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1481,13 +1508,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D37" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1495,12 +1522,26 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
         <v>143</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>144</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make F0AM tools work.
</commit_message>
<xml_diff>
--- a/Data/Functional_Group_SMARTs.xlsx
+++ b/Data/Functional_Group_SMARTs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3be239a439bc7664/Documents/Research/Projects/MIT/pOrgNO3/code/MCM_RCIM_SMILES/python/pyMCM/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{8C4F3C4E-712A-4552-94B7-A2C1FF83A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF2DC0EE-FA1E-4674-8A2A-3EC33138F8E7}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{8C4F3C4E-712A-4552-94B7-A2C1FF83A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3891CF8-45AF-4B5D-86FF-8031C275EB9C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{D7025BAE-6866-4008-AAF2-D095803B35C8}"/>
   </bookViews>
@@ -875,15 +875,15 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="51.140625" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="137.7109375" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="30.85546875" customWidth="1"/>
   </cols>

</xml_diff>